<commit_message>
Updated property views, inspections, property view page, install script, and more...
</commit_message>
<xml_diff>
--- a/Documentation/sprint2_suggested_work_by_jake.xlsx
+++ b/Documentation/sprint2_suggested_work_by_jake.xlsx
@@ -209,12 +209,6 @@
     <t>Developer</t>
   </si>
   <si>
-    <t>michael</t>
-  </si>
-  <si>
-    <t>jason</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Create a table </t>
     </r>
@@ -241,7 +235,13 @@
     </r>
   </si>
   <si>
-    <t>jake</t>
+    <t>Michael</t>
+  </si>
+  <si>
+    <t>Jason</t>
+  </si>
+  <si>
+    <t>Jake</t>
   </si>
 </sst>
 </file>
@@ -633,7 +633,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="E12" sqref="A1:E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,7 +674,7 @@
         <v>15</v>
       </c>
       <c r="E2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -689,7 +689,7 @@
         <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -701,10 +701,10 @@
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" t="s">
         <v>28</v>
-      </c>
-      <c r="E4" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -731,7 +731,7 @@
         <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -761,7 +761,7 @@
         <v>19</v>
       </c>
       <c r="E8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -776,7 +776,7 @@
         <v>20</v>
       </c>
       <c r="E9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -791,7 +791,7 @@
         <v>21</v>
       </c>
       <c r="E10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="60" x14ac:dyDescent="0.25">

</xml_diff>